<commit_message>
Added Asserter/LogicHooks to Excel compiler
</commit_message>
<xml_diff>
--- a/samples/scripting/Book1.xlsx
+++ b/samples/scripting/Book1.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9792" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9792"/>
   </bookViews>
   <sheets>
-    <sheet name="1-Schritt-Dialoge" sheetId="2" r:id="rId1"/>
-    <sheet name="2-Schritt-Dialoge" sheetId="3" r:id="rId2"/>
-    <sheet name="3-Schritt-Dialoge" sheetId="1" r:id="rId3"/>
+    <sheet name="Convos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>User</t>
   </si>
@@ -33,9 +31,6 @@
     <t>Nein</t>
   </si>
   <si>
-    <t>Troy</t>
-  </si>
-  <si>
     <t>Möchten Sie….?</t>
   </si>
   <si>
@@ -52,6 +47,17 @@
   </si>
   <si>
     <t>Rufen Sie an….</t>
+  </si>
+  <si>
+    <t>Bot</t>
+  </si>
+  <si>
+    <t>Möchten Sie….?
+PAUSE 1000</t>
+  </si>
+  <si>
+    <t>Was genau?
+BUTTONS Button1|Button2|Button3</t>
   </si>
 </sst>
 </file>
@@ -101,10 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,62 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="42.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="46.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -484,9 +441,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -494,9 +451,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>6</v>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -506,12 +463,12 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -521,22 +478,22 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>